<commit_message>
ADDED EXPONENT TO EXCEL
</commit_message>
<xml_diff>
--- a/RESULTATS.xlsx
+++ b/RESULTATS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acost\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{752DC563-8EB1-42A0-A745-27F80F85C5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EB854F-9CD9-4D0A-8A54-87BAE51DA55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{52C0F982-1B6C-40D1-99F9-1436615C1D22}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{52C0F982-1B6C-40D1-99F9-1436615C1D22}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>n</t>
   </si>
@@ -388,14 +388,25 @@
   </si>
   <si>
     <t>n: 83886080, k: 8, cost_mitja: 129291, variancia: 1,20382e+09, Std: 34696,1</t>
+  </si>
+  <si>
+    <t>EXPONENT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -423,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -433,6 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,7 +762,7 @@
   <dimension ref="B1:M107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,6 +791,9 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
@@ -798,6 +813,10 @@
         <f t="array" ref="F2:F106">_xlfn.TEXTAFTER(I2:I106,"Std: ")</f>
         <v>0,632456</v>
       </c>
+      <c r="G2">
+        <f>LOG(D2-LOG(B2)) / LOG(B2)</f>
+        <v>0.71600334363479923</v>
+      </c>
       <c r="I2" t="s">
         <v>5</v>
       </c>
@@ -819,7 +838,10 @@
       <c r="F3" s="1" t="str">
         <v>0,823273</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3">
+        <f>LOG(D3-LOG(B3)) / LOG(B3)</f>
+        <v>0.79934054945358168</v>
+      </c>
       <c r="I3" t="s">
         <v>6</v>
       </c>
@@ -841,7 +863,11 @@
       <c r="F4" s="1" t="str">
         <v>0,674949</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4">
+        <f t="shared" ref="G4:G67" si="1">LOG(D4-LOG(B4)) / LOG(B4)</f>
+        <v>0.86332286012045589</v>
+      </c>
+      <c r="H4" s="5"/>
       <c r="I4" t="s">
         <v>7</v>
       </c>
@@ -863,7 +889,10 @@
       <c r="F5" s="1" t="str">
         <v>0,316228</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0.89762709129044149</v>
+      </c>
       <c r="I5" t="s">
         <v>8</v>
       </c>
@@ -885,7 +914,10 @@
       <c r="F6" s="1" t="str">
         <v>0,316228</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.90848501887864974</v>
+      </c>
       <c r="I6" t="s">
         <v>9</v>
       </c>
@@ -907,7 +939,10 @@
       <c r="F7" s="1" t="str">
         <v>0,316228</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.90848501887864974</v>
+      </c>
       <c r="I7" t="s">
         <v>10</v>
       </c>
@@ -929,7 +964,10 @@
       <c r="F8" s="1" t="str">
         <v>0,316228</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.90848501887864974</v>
+      </c>
       <c r="I8" t="s">
         <v>11</v>
       </c>
@@ -951,7 +989,10 @@
       <c r="F9" s="1" t="str">
         <v>1,54919</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.62950979256578699</v>
+      </c>
       <c r="I9" t="s">
         <v>12</v>
       </c>
@@ -973,7 +1014,10 @@
       <c r="F10" s="1" t="str">
         <v>1,68655</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.7549403846982673</v>
+      </c>
       <c r="I10" t="s">
         <v>13</v>
       </c>
@@ -995,7 +1039,10 @@
       <c r="F11" s="1" t="str">
         <v>2,17307</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.84877995865896405</v>
+      </c>
       <c r="I11" t="s">
         <v>14</v>
       </c>
@@ -1017,7 +1064,10 @@
       <c r="F12" s="1" t="str">
         <v>2,00278</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0.89040220751410715</v>
+      </c>
       <c r="I12" t="s">
         <v>15</v>
       </c>
@@ -1039,7 +1089,10 @@
       <c r="F13" s="1" t="str">
         <v>0,788811</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.94118078912715986</v>
+      </c>
       <c r="I13" t="s">
         <v>16</v>
       </c>
@@ -1061,7 +1114,10 @@
       <c r="F14" s="1" t="str">
         <v>0,674949</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0.96145194321568972</v>
+      </c>
       <c r="I14" t="s">
         <v>17</v>
       </c>
@@ -1083,7 +1139,10 @@
       <c r="F15" s="1" t="str">
         <v>0,567646</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0.96609950253785548</v>
+      </c>
       <c r="I15" t="s">
         <v>18</v>
       </c>
@@ -1105,7 +1164,10 @@
       <c r="F16" s="1" t="str">
         <v>1,56702</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>0.5523181581278771</v>
+      </c>
       <c r="I16" t="s">
         <v>19</v>
       </c>
@@ -1127,7 +1189,10 @@
       <c r="F17" s="1" t="str">
         <v>4,19524</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0.68408267795104327</v>
+      </c>
       <c r="I17" t="s">
         <v>20</v>
       </c>
@@ -1149,7 +1214,10 @@
       <c r="F18" s="1" t="str">
         <v>4,87739</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>0.77890649880893104</v>
+      </c>
       <c r="I18" t="s">
         <v>21</v>
       </c>
@@ -1171,7 +1239,10 @@
       <c r="F19" s="1" t="str">
         <v>4,19524</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>0.84911388675192023</v>
+      </c>
       <c r="I19" t="s">
         <v>22</v>
       </c>
@@ -1193,7 +1264,10 @@
       <c r="F20" s="1" t="str">
         <v>6,73713</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>0.89581907222018564</v>
+      </c>
       <c r="I20" t="s">
         <v>23</v>
       </c>
@@ -1215,7 +1289,10 @@
       <c r="F21" s="1" t="str">
         <v>6,95701</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>0.93146590247497807</v>
+      </c>
       <c r="I21" t="s">
         <v>24</v>
       </c>
@@ -1237,7 +1314,10 @@
       <c r="F22" s="1" t="str">
         <v>7,09382</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>0.95432532641204992</v>
+      </c>
       <c r="I22" t="s">
         <v>25</v>
       </c>
@@ -1259,7 +1339,10 @@
       <c r="F23" s="1" t="str">
         <v>3,40588</v>
       </c>
-      <c r="G23" s="1"/>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>0.47692356604616565</v>
+      </c>
       <c r="I23" t="s">
         <v>26</v>
       </c>
@@ -1281,7 +1364,10 @@
       <c r="F24" s="1" t="str">
         <v>8,82484</v>
       </c>
-      <c r="G24" s="1"/>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>0.60634550853155578</v>
+      </c>
       <c r="I24" t="s">
         <v>27</v>
       </c>
@@ -1303,7 +1389,10 @@
       <c r="F25" s="1" t="str">
         <v>12,6842</v>
       </c>
-      <c r="G25" s="1"/>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>0.69501414112055693</v>
+      </c>
       <c r="I25" t="s">
         <v>28</v>
       </c>
@@ -1325,7 +1414,10 @@
       <c r="F26" s="1" t="str">
         <v>12,1198</v>
       </c>
-      <c r="G26" s="1"/>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>0.78660257286885182</v>
+      </c>
       <c r="I26" t="s">
         <v>29</v>
       </c>
@@ -1347,7 +1439,10 @@
       <c r="F27" s="1" t="str">
         <v>7,00793</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>0.83971681633340189</v>
+      </c>
       <c r="I27" t="s">
         <v>30</v>
       </c>
@@ -1369,7 +1464,10 @@
       <c r="F28" s="1" t="str">
         <v>17,0714</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>0.88845709185881516</v>
+      </c>
       <c r="I28" t="s">
         <v>31</v>
       </c>
@@ -1391,7 +1489,10 @@
       <c r="F29" s="1" t="str">
         <v>15,3275</v>
       </c>
-      <c r="G29" s="1"/>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>0.92476188086302114</v>
+      </c>
       <c r="I29" t="s">
         <v>32</v>
       </c>
@@ -1413,7 +1514,10 @@
       <c r="F30" s="1" t="str">
         <v>3,55903</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>0.42727064556647076</v>
+      </c>
       <c r="I30" t="s">
         <v>33</v>
       </c>
@@ -1435,7 +1539,10 @@
       <c r="F31" s="1" t="str">
         <v>7,44536</v>
       </c>
-      <c r="G31" s="1"/>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>0.52526441179110761</v>
+      </c>
       <c r="I31" t="s">
         <v>34</v>
       </c>
@@ -1457,7 +1564,10 @@
       <c r="F32" s="1" t="str">
         <v>17,7814</v>
       </c>
-      <c r="G32" s="1"/>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>0.63184660706808105</v>
+      </c>
       <c r="I32" t="s">
         <v>35</v>
       </c>
@@ -1479,7 +1589,10 @@
       <c r="F33" s="1" t="str">
         <v>28,358</v>
       </c>
-      <c r="G33" s="1"/>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>0.71837205830264228</v>
+      </c>
       <c r="I33" t="s">
         <v>36</v>
       </c>
@@ -1501,7 +1614,10 @@
       <c r="F34" s="1" t="str">
         <v>33,5301</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>0.78753830331320007</v>
+      </c>
       <c r="I34" t="s">
         <v>37</v>
       </c>
@@ -1523,7 +1639,10 @@
       <c r="F35" s="1" t="str">
         <v>48,4755</v>
       </c>
-      <c r="G35" s="1"/>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>0.83004033672825561</v>
+      </c>
       <c r="I35" t="s">
         <v>38</v>
       </c>
@@ -1545,7 +1664,10 @@
       <c r="F36" s="1" t="str">
         <v>80,3808</v>
       </c>
-      <c r="G36" s="1"/>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>0.88234163342185323</v>
+      </c>
       <c r="I36" t="s">
         <v>39</v>
       </c>
@@ -1567,7 +1689,10 @@
       <c r="F37" s="1" t="str">
         <v>3,3665</v>
       </c>
-      <c r="G37" s="1"/>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>0.37528618411157216</v>
+      </c>
       <c r="I37" t="s">
         <v>40</v>
       </c>
@@ -1589,7 +1714,10 @@
       <c r="F38" s="1" t="str">
         <v>11,4412</v>
       </c>
-      <c r="G38" s="1"/>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>0.48448959068236402</v>
+      </c>
       <c r="I38" t="s">
         <v>41</v>
       </c>
@@ -1611,7 +1739,10 @@
       <c r="F39" s="1" t="str">
         <v>32,3641</v>
       </c>
-      <c r="G39" s="1"/>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>0.59174552179480444</v>
+      </c>
       <c r="I39" t="s">
         <v>42</v>
       </c>
@@ -1633,7 +1764,10 @@
       <c r="F40" s="1" t="str">
         <v>72,3507</v>
       </c>
-      <c r="G40" s="1"/>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>0.67042082671781777</v>
+      </c>
       <c r="I40" t="s">
         <v>43</v>
       </c>
@@ -1655,7 +1789,10 @@
       <c r="F41" s="1" t="str">
         <v>87,4391</v>
       </c>
-      <c r="G41" s="1"/>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>0.73090477733468506</v>
+      </c>
       <c r="I41" t="s">
         <v>44</v>
       </c>
@@ -1677,7 +1814,10 @@
       <c r="F42" s="1" t="str">
         <v>218,212</v>
       </c>
-      <c r="G42" s="1"/>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>0.78774973317670494</v>
+      </c>
       <c r="I42" t="s">
         <v>45</v>
       </c>
@@ -1699,7 +1839,10 @@
       <c r="F43" s="1" t="str">
         <v>238,828</v>
       </c>
-      <c r="G43" s="1"/>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>0.83642566090293735</v>
+      </c>
       <c r="I43" t="s">
         <v>46</v>
       </c>
@@ -1721,7 +1864,10 @@
       <c r="F44" s="1" t="str">
         <v>7,61285</v>
       </c>
-      <c r="G44" s="1"/>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>0.35542832179566203</v>
+      </c>
       <c r="I44" t="s">
         <v>47</v>
       </c>
@@ -1743,7 +1889,10 @@
       <c r="F45" s="1" t="str">
         <v>20,1784</v>
       </c>
-      <c r="G45" s="1"/>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>0.44503170117721302</v>
+      </c>
       <c r="I45" t="s">
         <v>48</v>
       </c>
@@ -1765,7 +1914,10 @@
       <c r="F46" s="1" t="str">
         <v>38,735</v>
       </c>
-      <c r="G46" s="1"/>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>0.54722320285552417</v>
+      </c>
       <c r="I46" t="s">
         <v>49</v>
       </c>
@@ -1787,7 +1939,10 @@
       <c r="F47" s="1" t="str">
         <v>71,0963</v>
       </c>
-      <c r="G47" s="1"/>
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>0.61644958643187997</v>
+      </c>
       <c r="I47" t="s">
         <v>50</v>
       </c>
@@ -1809,7 +1964,10 @@
       <c r="F48" s="1" t="str">
         <v>220,259</v>
       </c>
-      <c r="G48" s="1"/>
+      <c r="G48">
+        <f t="shared" si="1"/>
+        <v>0.69277224079415822</v>
+      </c>
       <c r="I48" t="s">
         <v>51</v>
       </c>
@@ -1831,7 +1989,10 @@
       <c r="F49" s="1" t="str">
         <v>301,486</v>
       </c>
-      <c r="G49" s="1"/>
+      <c r="G49">
+        <f t="shared" si="1"/>
+        <v>0.74418610503685323</v>
+      </c>
       <c r="I49" t="s">
         <v>52</v>
       </c>
@@ -1853,7 +2014,10 @@
       <c r="F50" s="1" t="str">
         <v>569,618</v>
       </c>
-      <c r="G50" s="1"/>
+      <c r="G50">
+        <f t="shared" si="1"/>
+        <v>0.79591403961433405</v>
+      </c>
       <c r="I50" t="s">
         <v>53</v>
       </c>
@@ -1875,7 +2039,10 @@
       <c r="F51" s="1" t="str">
         <v>4,54117</v>
       </c>
-      <c r="G51" s="1"/>
+      <c r="G51">
+        <f t="shared" si="1"/>
+        <v>0.32169932364278248</v>
+      </c>
       <c r="I51" t="s">
         <v>54</v>
       </c>
@@ -1897,7 +2064,10 @@
       <c r="F52" s="1" t="str">
         <v>25,629</v>
       </c>
-      <c r="G52" s="1"/>
+      <c r="G52">
+        <f t="shared" si="1"/>
+        <v>0.41012671477477469</v>
+      </c>
       <c r="I52" t="s">
         <v>55</v>
       </c>
@@ -1919,7 +2089,10 @@
       <c r="F53" s="1" t="str">
         <v>74,9801</v>
       </c>
-      <c r="G53" s="1"/>
+      <c r="G53">
+        <f t="shared" si="1"/>
+        <v>0.49409904746473116</v>
+      </c>
       <c r="I53" t="s">
         <v>56</v>
       </c>
@@ -1941,7 +2114,10 @@
       <c r="F54" s="1" t="str">
         <v>189,703</v>
       </c>
-      <c r="G54" s="1"/>
+      <c r="G54">
+        <f t="shared" si="1"/>
+        <v>0.58089933839718833</v>
+      </c>
       <c r="I54" t="s">
         <v>57</v>
       </c>
@@ -1963,7 +2139,10 @@
       <c r="F55" s="1" t="str">
         <v>557,802</v>
       </c>
-      <c r="G55" s="1"/>
+      <c r="G55">
+        <f t="shared" si="1"/>
+        <v>0.65531491289521748</v>
+      </c>
       <c r="I55" t="s">
         <v>58</v>
       </c>
@@ -1985,7 +2164,10 @@
       <c r="F56" s="1" t="str">
         <v>794,577</v>
       </c>
-      <c r="G56" s="1"/>
+      <c r="G56">
+        <f t="shared" si="1"/>
+        <v>0.70424968175857272</v>
+      </c>
       <c r="I56" t="s">
         <v>59</v>
       </c>
@@ -2007,7 +2189,10 @@
       <c r="F57" s="1" t="str">
         <v>1602,36</v>
       </c>
-      <c r="G57" s="1"/>
+      <c r="G57">
+        <f t="shared" si="1"/>
+        <v>0.75660970336114031</v>
+      </c>
       <c r="I57" t="s">
         <v>60</v>
       </c>
@@ -2029,7 +2214,10 @@
       <c r="F58" s="1" t="str">
         <v>19,1787</v>
       </c>
-      <c r="G58" s="1"/>
+      <c r="G58">
+        <f t="shared" si="1"/>
+        <v>0.30885690455895876</v>
+      </c>
       <c r="I58" t="s">
         <v>61</v>
       </c>
@@ -2051,7 +2239,10 @@
       <c r="F59" s="1" t="str">
         <v>59,6598</v>
       </c>
-      <c r="G59" s="1"/>
+      <c r="G59">
+        <f t="shared" si="1"/>
+        <v>0.39648983111038827</v>
+      </c>
       <c r="I59" t="s">
         <v>62</v>
       </c>
@@ -2073,7 +2264,10 @@
       <c r="F60" s="1" t="str">
         <v>106,944</v>
       </c>
-      <c r="G60" s="1"/>
+      <c r="G60">
+        <f t="shared" si="1"/>
+        <v>0.4774330277673291</v>
+      </c>
       <c r="I60" t="s">
         <v>63</v>
       </c>
@@ -2095,7 +2289,10 @@
       <c r="F61" s="1" t="str">
         <v>608,426</v>
       </c>
-      <c r="G61" s="1"/>
+      <c r="G61">
+        <f t="shared" si="1"/>
+        <v>0.56008902922159742</v>
+      </c>
       <c r="I61" t="s">
         <v>64</v>
       </c>
@@ -2117,7 +2314,10 @@
       <c r="F62" s="1" t="str">
         <v>1049,77</v>
       </c>
-      <c r="G62" s="1"/>
+      <c r="G62">
+        <f t="shared" si="1"/>
+        <v>0.62571777605947732</v>
+      </c>
       <c r="I62" t="s">
         <v>65</v>
       </c>
@@ -2139,7 +2339,10 @@
       <c r="F63" s="1" t="str">
         <v>1601,18</v>
       </c>
-      <c r="G63" s="1"/>
+      <c r="G63">
+        <f t="shared" si="1"/>
+        <v>0.68090004593102826</v>
+      </c>
       <c r="I63" t="s">
         <v>66</v>
       </c>
@@ -2161,7 +2364,10 @@
       <c r="F64" s="1" t="str">
         <v>2135,29</v>
       </c>
-      <c r="G64" s="1"/>
+      <c r="G64">
+        <f t="shared" si="1"/>
+        <v>0.72753204942369398</v>
+      </c>
       <c r="I64" t="s">
         <v>67</v>
       </c>
@@ -2183,7 +2389,10 @@
       <c r="F65" s="1" t="str">
         <v>55,4981</v>
       </c>
-      <c r="G65" s="1"/>
+      <c r="G65">
+        <f t="shared" si="1"/>
+        <v>0.30058614762088143</v>
+      </c>
       <c r="I65" t="s">
         <v>68</v>
       </c>
@@ -2205,7 +2414,10 @@
       <c r="F66" s="1" t="str">
         <v>82,9651</v>
       </c>
-      <c r="G66" s="1"/>
+      <c r="G66">
+        <f t="shared" si="1"/>
+        <v>0.3791734889611173</v>
+      </c>
       <c r="I66" t="s">
         <v>69</v>
       </c>
@@ -2227,7 +2439,10 @@
       <c r="F67" s="1" t="str">
         <v>1043,35</v>
       </c>
-      <c r="G67" s="1"/>
+      <c r="G67">
+        <f t="shared" si="1"/>
+        <v>0.48305409701869623</v>
+      </c>
       <c r="I67" t="s">
         <v>70</v>
       </c>
@@ -2243,13 +2458,16 @@
         <v>2267.1999999999998</v>
       </c>
       <c r="E68">
-        <f t="shared" ref="E68:E106" si="1">F68*F68</f>
+        <f t="shared" ref="E68:E106" si="2">F68*F68</f>
         <v>270063.14497600007</v>
       </c>
       <c r="F68" s="1" t="str">
         <v>519,676</v>
       </c>
-      <c r="G68" s="1"/>
+      <c r="G68">
+        <f t="shared" ref="G68:G106" si="3">LOG(D68-LOG(B68)) / LOG(B68)</f>
+        <v>0.52258903485850472</v>
+      </c>
       <c r="I68" t="s">
         <v>71</v>
       </c>
@@ -2265,13 +2483,16 @@
         <v>6322.6</v>
       </c>
       <c r="E69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2856877.4528999999</v>
       </c>
       <c r="F69" s="1" t="str">
         <v>1690,23</v>
       </c>
-      <c r="G69" s="1"/>
+      <c r="G69">
+        <f t="shared" si="3"/>
+        <v>0.59210578180497275</v>
+      </c>
       <c r="I69" t="s">
         <v>72</v>
       </c>
@@ -2287,13 +2508,16 @@
         <v>14481</v>
       </c>
       <c r="E70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18759639.937599998</v>
       </c>
       <c r="F70" s="1" t="str">
         <v>4331,24</v>
       </c>
-      <c r="G70" s="1"/>
+      <c r="G70">
+        <f t="shared" si="3"/>
+        <v>0.64821689439130026</v>
+      </c>
       <c r="I70" t="s">
         <v>73</v>
       </c>
@@ -2309,13 +2533,16 @@
         <v>29990.5</v>
       </c>
       <c r="E71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43845983.856899999</v>
       </c>
       <c r="F71" s="1" t="str">
         <v>6621,63</v>
       </c>
-      <c r="G71" s="1"/>
+      <c r="G71">
+        <f t="shared" si="3"/>
+        <v>0.69749363617411209</v>
+      </c>
       <c r="I71" t="s">
         <v>74</v>
       </c>
@@ -2331,13 +2558,16 @@
         <v>77.8</v>
       </c>
       <c r="E72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>309.95715135999995</v>
       </c>
       <c r="F72" s="1" t="str">
         <v>17,6056</v>
       </c>
-      <c r="G72" s="1"/>
+      <c r="G72">
+        <f t="shared" si="3"/>
+        <v>0.27557567963510765</v>
+      </c>
       <c r="I72" t="s">
         <v>75</v>
       </c>
@@ -2353,13 +2583,16 @@
         <v>256.89999999999998</v>
       </c>
       <c r="E73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2098.3178947599999</v>
       </c>
       <c r="F73" s="1" t="str">
         <v>45,8074</v>
       </c>
-      <c r="G73" s="1"/>
+      <c r="G73">
+        <f t="shared" si="3"/>
+        <v>0.35690577881899771</v>
+      </c>
       <c r="I73" t="s">
         <v>76</v>
       </c>
@@ -2375,13 +2608,16 @@
         <v>853.4</v>
       </c>
       <c r="E74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>179612.37324900003</v>
       </c>
       <c r="F74" s="1" t="str">
         <v>423,807</v>
       </c>
-      <c r="G74" s="1"/>
+      <c r="G74">
+        <f t="shared" si="3"/>
+        <v>0.43570043285956012</v>
+      </c>
       <c r="I74" t="s">
         <v>77</v>
       </c>
@@ -2397,13 +2633,16 @@
         <v>2862.9</v>
       </c>
       <c r="E75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>913924.52803600009</v>
       </c>
       <c r="F75" s="1" t="str">
         <v>955,994</v>
       </c>
-      <c r="G75" s="1"/>
+      <c r="G75">
+        <f t="shared" si="3"/>
+        <v>0.51428672988117441</v>
+      </c>
       <c r="I75" t="s">
         <v>78</v>
       </c>
@@ -2419,13 +2658,16 @@
         <v>8356.7000000000007</v>
       </c>
       <c r="E76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15102084.099599998</v>
       </c>
       <c r="F76" s="1" t="str">
         <v>3886,14</v>
       </c>
-      <c r="G76" s="1"/>
+      <c r="G76">
+        <f t="shared" si="3"/>
+        <v>0.58362149746286407</v>
+      </c>
       <c r="I76" t="s">
         <v>79</v>
       </c>
@@ -2441,13 +2683,16 @@
         <v>16730.3</v>
       </c>
       <c r="E77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6942381.825600001</v>
       </c>
       <c r="F77" s="1" t="str">
         <v>2634,84</v>
       </c>
-      <c r="G77" s="1"/>
+      <c r="G77">
+        <f t="shared" si="3"/>
+        <v>0.62851184152972306</v>
+      </c>
       <c r="I77" t="s">
         <v>80</v>
       </c>
@@ -2463,13 +2708,16 @@
         <v>40495.699999999997</v>
       </c>
       <c r="E78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>186844294.81</v>
       </c>
       <c r="F78" s="1" t="str">
         <v>13669,1</v>
       </c>
-      <c r="G78" s="1"/>
+      <c r="G78">
+        <f t="shared" si="3"/>
+        <v>0.68565948375313956</v>
+      </c>
       <c r="I78" t="s">
         <v>81</v>
       </c>
@@ -2485,13 +2733,16 @@
         <v>94.2</v>
       </c>
       <c r="E79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>368.39811968999999</v>
       </c>
       <c r="F79" s="1" t="str">
         <v>19,1937</v>
       </c>
-      <c r="G79" s="1"/>
+      <c r="G79">
+        <f t="shared" si="3"/>
+        <v>0.27638861352613581</v>
+      </c>
       <c r="I79" t="s">
         <v>82</v>
       </c>
@@ -2507,13 +2758,16 @@
         <v>319</v>
       </c>
       <c r="E80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10690.526024999999</v>
       </c>
       <c r="F80" s="1" t="str">
         <v>103,395</v>
       </c>
-      <c r="G80" s="1"/>
+      <c r="G80">
+        <f t="shared" si="3"/>
+        <v>0.35525823283324198</v>
+      </c>
       <c r="I80" t="s">
         <v>83</v>
       </c>
@@ -2529,13 +2783,16 @@
         <v>921</v>
       </c>
       <c r="E81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39415.352088999993</v>
       </c>
       <c r="F81" s="1" t="str">
         <v>198,533</v>
       </c>
-      <c r="G81" s="1"/>
+      <c r="G81">
+        <f t="shared" si="3"/>
+        <v>0.42174977124215229</v>
+      </c>
       <c r="I81" t="s">
         <v>84</v>
       </c>
@@ -2551,13 +2808,16 @@
         <v>3791</v>
       </c>
       <c r="E82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1079043.1129000001</v>
       </c>
       <c r="F82" s="1" t="str">
         <v>1038,77</v>
       </c>
-      <c r="G82" s="1"/>
+      <c r="G82">
+        <f t="shared" si="3"/>
+        <v>0.5096357587159126</v>
+      </c>
       <c r="I82" t="s">
         <v>85</v>
       </c>
@@ -2573,13 +2833,16 @@
         <v>10828.8</v>
       </c>
       <c r="E83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9142882.6383999996</v>
       </c>
       <c r="F83" s="1" t="str">
         <v>3023,72</v>
       </c>
-      <c r="G83" s="1"/>
+      <c r="G83">
+        <f t="shared" si="3"/>
+        <v>0.57463731397732509</v>
+      </c>
       <c r="I83" t="s">
         <v>86</v>
       </c>
@@ -2595,13 +2858,16 @@
         <v>29191</v>
       </c>
       <c r="E84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65047289.736099996</v>
       </c>
       <c r="F84" s="1" t="str">
         <v>8065,19</v>
       </c>
-      <c r="G84" s="1"/>
+      <c r="G84">
+        <f t="shared" si="3"/>
+        <v>0.63600611988297107</v>
+      </c>
       <c r="I84" t="s">
         <v>87</v>
       </c>
@@ -2617,13 +2883,16 @@
         <v>52059.1</v>
       </c>
       <c r="E85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110874582.09000002</v>
       </c>
       <c r="F85" s="1" t="str">
         <v>10529,7</v>
       </c>
-      <c r="G85" s="1"/>
+      <c r="G85">
+        <f t="shared" si="3"/>
+        <v>0.67179986637108902</v>
+      </c>
       <c r="I85" t="s">
         <v>88</v>
       </c>
@@ -2639,13 +2908,16 @@
         <v>92.9</v>
       </c>
       <c r="E86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>483.87680783999997</v>
       </c>
       <c r="F86" s="1" t="str">
         <v>21,9972</v>
       </c>
-      <c r="G86" s="1"/>
+      <c r="G86">
+        <f t="shared" si="3"/>
+        <v>0.26392538748486172</v>
+      </c>
       <c r="I86" t="s">
         <v>89</v>
       </c>
@@ -2661,13 +2933,16 @@
         <v>399.2</v>
       </c>
       <c r="E87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>89288.611344000004</v>
       </c>
       <c r="F87" s="1" t="str">
         <v>298,812</v>
       </c>
-      <c r="G87" s="1"/>
+      <c r="G87">
+        <f t="shared" si="3"/>
+        <v>0.35417677829987571</v>
+      </c>
       <c r="I87" t="s">
         <v>90</v>
       </c>
@@ -2683,13 +2958,16 @@
         <v>1291.3</v>
       </c>
       <c r="E88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>228716.36704899999</v>
       </c>
       <c r="F88" s="1" t="str">
         <v>478,243</v>
       </c>
-      <c r="G88" s="1"/>
+      <c r="G88">
+        <f t="shared" si="3"/>
+        <v>0.42457181615657186</v>
+      </c>
       <c r="I88" t="s">
         <v>91</v>
       </c>
@@ -2705,13 +2983,16 @@
         <v>4364.8999999999996</v>
       </c>
       <c r="E89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2270355.8328999998</v>
       </c>
       <c r="F89" s="1" t="str">
         <v>1506,77</v>
       </c>
-      <c r="G89" s="1"/>
+      <c r="G89">
+        <f t="shared" si="3"/>
+        <v>0.49705396910294508</v>
+      </c>
       <c r="I89" t="s">
         <v>92</v>
       </c>
@@ -2727,13 +3008,16 @@
         <v>11307.6</v>
       </c>
       <c r="E90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10031599.252900001</v>
       </c>
       <c r="F90" s="1" t="str">
         <v>3167,27</v>
       </c>
-      <c r="G90" s="1"/>
+      <c r="G90">
+        <f t="shared" si="3"/>
+        <v>0.55357744005024689</v>
+      </c>
       <c r="I90" t="s">
         <v>93</v>
       </c>
@@ -2755,7 +3039,10 @@
       <c r="F91" s="1" t="str">
         <v>10044,9</v>
       </c>
-      <c r="G91" s="1"/>
+      <c r="G91">
+        <f t="shared" si="3"/>
+        <v>0.6155402174831881</v>
+      </c>
       <c r="I91" t="s">
         <v>94</v>
       </c>
@@ -2771,13 +3058,16 @@
         <v>80861.899999999994</v>
       </c>
       <c r="E92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>984503578.24000001</v>
       </c>
       <c r="F92" s="1" t="str">
         <v>31376,8</v>
       </c>
-      <c r="G92" s="1"/>
+      <c r="G92">
+        <f t="shared" si="3"/>
+        <v>0.67030219743273201</v>
+      </c>
       <c r="I92" t="s">
         <v>95</v>
       </c>
@@ -2793,13 +3083,16 @@
         <v>137.6</v>
       </c>
       <c r="E93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5460.4858040099998</v>
       </c>
       <c r="F93" s="1" t="str">
         <v>73,8951</v>
       </c>
-      <c r="G93" s="1"/>
+      <c r="G93">
+        <f t="shared" si="3"/>
+        <v>0.27731365056448526</v>
+      </c>
       <c r="I93" t="s">
         <v>96</v>
       </c>
@@ -2815,13 +3108,16 @@
         <v>318.5</v>
       </c>
       <c r="E94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12210.25</v>
       </c>
       <c r="F94" s="1" t="str">
         <v>110,5</v>
       </c>
-      <c r="G94" s="1"/>
+      <c r="G94">
+        <f t="shared" si="3"/>
+        <v>0.32699728160351782</v>
+      </c>
       <c r="I94" t="s">
         <v>97</v>
       </c>
@@ -2837,13 +3133,16 @@
         <v>1448.6</v>
       </c>
       <c r="E95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116221.67356900001</v>
       </c>
       <c r="F95" s="1" t="str">
         <v>340,913</v>
       </c>
-      <c r="G95" s="1"/>
+      <c r="G95">
+        <f t="shared" si="3"/>
+        <v>0.41437728968022758</v>
+      </c>
       <c r="I95" t="s">
         <v>98</v>
       </c>
@@ -2859,13 +3158,16 @@
         <v>5724.6</v>
       </c>
       <c r="E96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8736517.1776000019</v>
       </c>
       <c r="F96" s="1" t="str">
         <v>2955,76</v>
       </c>
-      <c r="G96" s="1"/>
+      <c r="G96">
+        <f t="shared" si="3"/>
+        <v>0.49289441190599886</v>
+      </c>
       <c r="I96" t="s">
         <v>99</v>
       </c>
@@ -2881,13 +3183,16 @@
         <v>11330.2</v>
       </c>
       <c r="E97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7605626.3088999996</v>
       </c>
       <c r="F97" s="1" t="str">
         <v>2757,83</v>
       </c>
-      <c r="G97" s="1"/>
+      <c r="G97">
+        <f t="shared" si="3"/>
+        <v>0.53182817370749447</v>
+      </c>
       <c r="I97" t="s">
         <v>100</v>
       </c>
@@ -2903,13 +3208,16 @@
         <v>41384.9</v>
       </c>
       <c r="E98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>301821129</v>
       </c>
       <c r="F98" s="1" t="str">
         <v>17373</v>
       </c>
-      <c r="G98" s="1"/>
+      <c r="G98">
+        <f t="shared" si="3"/>
+        <v>0.60566284841520646</v>
+      </c>
       <c r="I98" t="s">
         <v>101</v>
       </c>
@@ -2925,13 +3233,16 @@
         <v>97259.5</v>
       </c>
       <c r="E99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1132174444.8400002</v>
       </c>
       <c r="F99" s="1" t="str">
         <v>33647,8</v>
       </c>
-      <c r="G99" s="1"/>
+      <c r="G99">
+        <f t="shared" si="3"/>
+        <v>0.65435137551382272</v>
+      </c>
       <c r="I99" t="s">
         <v>102</v>
       </c>
@@ -2947,13 +3258,16 @@
         <v>168</v>
       </c>
       <c r="E100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35480.243043999995</v>
       </c>
       <c r="F100" s="1" t="str">
         <v>188,362</v>
       </c>
-      <c r="G100" s="1"/>
+      <c r="G100">
+        <f t="shared" si="3"/>
+        <v>0.27819451450223448</v>
+      </c>
       <c r="I100" t="s">
         <v>103</v>
       </c>
@@ -2969,13 +3283,16 @@
         <v>428.9</v>
       </c>
       <c r="E101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65046.421763999999</v>
       </c>
       <c r="F101" s="1" t="str">
         <v>255,042</v>
       </c>
-      <c r="G101" s="1"/>
+      <c r="G101">
+        <f t="shared" si="3"/>
+        <v>0.33119136288638612</v>
+      </c>
       <c r="I101" t="s">
         <v>104</v>
       </c>
@@ -2991,13 +3308,16 @@
         <v>1794.6</v>
       </c>
       <c r="E102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>850131.94467599993</v>
       </c>
       <c r="F102" s="1" t="str">
         <v>922,026</v>
       </c>
-      <c r="G102" s="1"/>
+      <c r="G102">
+        <f t="shared" si="3"/>
+        <v>0.41042063987580046</v>
+      </c>
       <c r="I102" t="s">
         <v>105</v>
       </c>
@@ -3013,13 +3333,16 @@
         <v>5193.8</v>
       </c>
       <c r="E103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11150123.072399998</v>
       </c>
       <c r="F103" s="1" t="str">
         <v>3339,18</v>
       </c>
-      <c r="G103" s="1"/>
+      <c r="G103">
+        <f t="shared" si="3"/>
+        <v>0.46882477744880519</v>
+      </c>
       <c r="I103" t="s">
         <v>106</v>
       </c>
@@ -3035,13 +3358,16 @@
         <v>21447</v>
       </c>
       <c r="E104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67563961.2729</v>
       </c>
       <c r="F104" s="1" t="str">
         <v>8219,73</v>
       </c>
-      <c r="G104" s="1"/>
+      <c r="G104">
+        <f t="shared" si="3"/>
+        <v>0.54661478738017322</v>
+      </c>
       <c r="I104" t="s">
         <v>107</v>
       </c>
@@ -3057,13 +3383,16 @@
         <v>50617.4</v>
       </c>
       <c r="E105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>318012322.41000003</v>
       </c>
       <c r="F105" s="1" t="str">
         <v>17832,9</v>
       </c>
-      <c r="G105" s="1"/>
+      <c r="G105">
+        <f t="shared" si="3"/>
+        <v>0.59369206803979757</v>
+      </c>
       <c r="I105" t="s">
         <v>108</v>
       </c>
@@ -3079,13 +3408,16 @@
         <v>129291</v>
       </c>
       <c r="E106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1203819355.2099998</v>
       </c>
       <c r="F106" s="1" t="str">
         <v>34696,1</v>
       </c>
-      <c r="G106" s="1"/>
+      <c r="G106">
+        <f t="shared" si="3"/>
+        <v>0.64509612844393416</v>
+      </c>
       <c r="I106" t="s">
         <v>109</v>
       </c>

</xml_diff>